<commit_message>
Creating DatenBank with all coordinates of Bus Station
</commit_message>
<xml_diff>
--- a/TestResult.xlsx
+++ b/TestResult.xlsx
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>52.1667298</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>9.906213299999999</v>
       </c>
     </row>
     <row r="3">

</xml_diff>